<commit_message>
PCB Model Final (hoffentlich)
</commit_message>
<xml_diff>
--- a/2.2 Measurement Chain/signal-conditioning_calc-2.xlsx
+++ b/2.2 Measurement Chain/signal-conditioning_calc-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\HSRW\Semester 5\Group Project\Group-Project_WS2526\2.2 Measurement Chain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAE95E3-1AC1-4698-BE8F-4CCD8F8B9A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0061359-31FC-436D-96C8-92E2339EA557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
   <si>
     <t xml:space="preserve">Using INA gain of </t>
   </si>
@@ -139,9 +139,6 @@
     <t>Total I_typ</t>
   </si>
   <si>
-    <t>LDO</t>
-  </si>
-  <si>
     <t>Total I_max</t>
   </si>
   <si>
@@ -228,6 +225,15 @@
   <si>
     <t>I @10V [mA]</t>
   </si>
+  <si>
+    <t>Total I_spec</t>
+  </si>
+  <si>
+    <t>Estimate Spec [h]</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
 </sst>
 </file>
 
@@ -284,7 +290,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -396,11 +402,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -463,6 +478,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3882,7 +3899,7 @@
   <dimension ref="A1:K996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3931,117 +3948,120 @@
       <c r="C2" s="1">
         <v>28.57</v>
       </c>
-      <c r="D2" s="27"/>
+      <c r="D2" s="27">
+        <f>AVERAGE(B2:C2)</f>
+        <v>21.425000000000001</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H2" s="1">
-        <f>SUM(B2:B96)</f>
-        <v>655.77</v>
+        <f>SUM($B$2:$B$96)</f>
+        <v>653.27</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="K2" s="1">
-        <f>SUM(B3:B8)</f>
-        <v>9.0710000000000015</v>
+        <f>SUM(B3:B7)</f>
+        <v>4.0709999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D3" s="27">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="1">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>6</v>
-      </c>
-      <c r="D3" s="27">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="H3" s="1">
-        <f>SUM(C2:C96)</f>
-        <v>671.90769999999998</v>
+        <f>SUM($C$2:$C$96)</f>
+        <v>1265.9077</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" s="1">
-        <f>SUM(C3:C8)</f>
-        <v>10.822000000000001</v>
+        <f>SUM(C3:C7)</f>
+        <v>4.8219999999999992</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
+        <v>0.45</v>
       </c>
       <c r="C4" s="1">
-        <v>2.2999999999999998</v>
+        <v>0.51</v>
       </c>
       <c r="D4" s="27">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="1">
+        <f>SUM($D$2:$D$97)</f>
+        <v>665.00199999999984</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="1">
-        <v>5000</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="K4" s="1">
-        <f>SUM(D3:D8)</f>
-        <v>14.005000000000001</v>
+        <f>SUM(D3:D7)</f>
+        <v>8.004999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" s="1">
-        <v>0.45</v>
+        <v>1E-3</v>
       </c>
       <c r="C5" s="1">
-        <v>0.51</v>
+        <v>2E-3</v>
       </c>
       <c r="D5" s="27">
-        <v>1</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H5" s="1">
-        <f>H4/H3</f>
-        <v>7.4414982891251285</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1">
-        <v>1E-3</v>
+        <v>1.24</v>
       </c>
       <c r="C6" s="1">
-        <v>2E-3</v>
+        <v>1.43</v>
       </c>
       <c r="D6" s="27">
-        <v>5.0000000000000001E-3</v>
+        <v>3</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H6" s="1">
-        <f>H4/H2</f>
-        <v>7.6246244872440032</v>
+        <f>$H5/(H3*1.2)</f>
+        <v>4.6080242132450362</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4049,13 +4069,20 @@
         <v>42</v>
       </c>
       <c r="B7" s="1">
-        <v>1.24</v>
+        <v>0.38</v>
       </c>
       <c r="C7" s="1">
-        <v>1.43</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D7" s="27">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="1">
+        <f>$H5/(H2*1.2)</f>
+        <v>8.929437037263817</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4063,102 +4090,169 @@
         <v>43</v>
       </c>
       <c r="B8" s="1">
-        <v>0.38</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.57999999999999996</v>
+        <v>500</v>
+      </c>
+      <c r="C8">
+        <v>600</v>
       </c>
       <c r="D8" s="27">
-        <v>1</v>
+        <v>500</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8">
+        <f>$H5/(H4*1.2)</f>
+        <v>8.7719034428969156</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="1">
-        <v>500</v>
-      </c>
-      <c r="C9" s="35">
-        <v>500</v>
-      </c>
-      <c r="D9" s="27"/>
+      <c r="B9" s="28">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D9" s="27">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="28">
-        <v>2.2999999999999998</v>
+      <c r="B10" s="1">
+        <v>1E-3</v>
       </c>
       <c r="C10" s="1">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D10" s="27"/>
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="D10" s="27">
+        <v>2E-3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="1">
+        <f>SUM($B$2:$B$96)</f>
+        <v>653.27</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="1">
-        <v>1E-3</v>
+      <c r="B11" s="28">
+        <v>0.10100000000000001</v>
       </c>
       <c r="C11" s="1">
-        <v>2.7000000000000001E-3</v>
-      </c>
-      <c r="D11" s="27"/>
+        <v>0.183</v>
+      </c>
+      <c r="D11" s="27">
+        <v>0.15</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="1">
+        <f>SUM($C$2:$C$96)</f>
+        <v>1265.9077</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="28">
-        <v>0.10100000000000001</v>
+      <c r="B12" s="1">
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="C12" s="1">
-        <v>0.183</v>
-      </c>
-      <c r="D12" s="27"/>
+        <v>0.03</v>
+      </c>
+      <c r="D12" s="27">
+        <v>0.02</v>
+      </c>
+      <c r="G12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="1">
+        <f>SUM($D$2:$D$97)</f>
+        <v>665.00199999999984</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B13" s="1">
-        <v>1.7000000000000001E-2</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="D13" s="27"/>
+        <v>10</v>
+      </c>
+      <c r="D13" s="27">
+        <v>10</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="1">
+        <v>5000</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="1">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="C14" s="1">
-        <v>10</v>
-      </c>
-      <c r="D14" s="27"/>
+        <v>120</v>
+      </c>
+      <c r="D14" s="27">
+        <v>120</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="1">
+        <f>$H13/(H11*1.2)</f>
+        <v>3.2914458666035973</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="1">
-        <v>120</v>
-      </c>
-      <c r="C15" s="1">
-        <v>120</v>
-      </c>
-      <c r="D15" s="27"/>
+        <v>64</v>
+      </c>
+      <c r="B15" s="37">
+        <v>2.5</v>
+      </c>
+      <c r="C15" s="35">
+        <v>500</v>
+      </c>
+      <c r="D15" s="27">
+        <v>2.9</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="1">
+        <f>$H13/(H10*1.2)</f>
+        <v>6.3781693123312975</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
-      <c r="D16" s="27"/>
+      <c r="G16" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16">
+        <f>$H13/(H12*1.2)</f>
+        <v>6.2656453163549406</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="27"/>
@@ -8107,15 +8201,15 @@
         <v>25</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1">
         <v>5.0118700000000005E-4</v>
@@ -8126,7 +8220,7 @@
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1">
         <v>7.0000000000000007E-2</v>
@@ -8135,7 +8229,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" s="1">
         <f>((B2+B3)*C3+B4)*C4 + B5 +B6</f>
@@ -8144,7 +8238,7 @@
     </row>
     <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1">
         <v>0.25</v>
@@ -8153,7 +8247,7 @@
         <v>4.26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F4" s="1">
         <f>5000000/F3</f>
@@ -8162,7 +8256,7 @@
     </row>
     <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1">
         <v>6.3954000000000004</v>
@@ -8171,7 +8265,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="1">
         <f>LOG(F4,2)</f>
@@ -8180,7 +8274,7 @@
     </row>
     <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="1">
         <v>2.85</v>
@@ -12187,7 +12281,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -16242,13 +16336,13 @@
         <v>4</v>
       </c>
       <c r="B1" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="26" t="s">
         <v>61</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>